<commit_message>
"Converting excel data to pojo to send it as payload.And generating id based on instructions given in the Id column."
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CreateUserData.xlsx
+++ b/src/test/resources/testdata/CreateUserData.xlsx
@@ -20,42 +20,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
-  <si>
-    <t xml:space="preserve">ID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Country</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+  <si>
+    <t xml:space="preserve">Id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UserName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FirstName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LastName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">john.doe</t>
   </si>
   <si>
     <t xml:space="preserve">John</t>
   </si>
   <si>
-    <t xml:space="preserve">USA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tao Chain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chaina</t>
+    <t xml:space="preserve">Doe</t>
+  </si>
+  <si>
+    <t xml:space="preserve">johndoe@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">toa.chan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tao </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taochain@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">husain.k</t>
   </si>
   <si>
     <t xml:space="preserve">Md. Husain</t>
   </si>
   <si>
-    <t xml:space="preserve">India</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vankat Iyar</t>
+    <t xml:space="preserve">Ahmed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">husain@outlook.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vankat.iyar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vankat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Iyar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">vankat@yahoo.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helen.kip</t>
   </si>
   <si>
     <t xml:space="preserve">Helen</t>
   </si>
   <si>
-    <t xml:space="preserve">UK</t>
+    <t xml:space="preserve">Kip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">helen@ukmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H12345678</t>
   </si>
 </sst>
 </file>
@@ -65,11 +125,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -85,6 +146,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0000FF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -129,8 +197,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -151,81 +227,163 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.94"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="0" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="n">
+      <c r="A2" s="1" t="n">
         <v>1001</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="0" t="s">
-        <v>4</v>
+        <v>7</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>9876543210</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
+      <c r="A3" s="1" t="n">
         <v>1002</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>6</v>
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="0" t="n">
+        <v>8765432109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
+      <c r="A4" s="1" t="n">
         <v>1003</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" s="0" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="0" t="n">
+        <v>7654321098</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
+      <c r="A5" s="1" t="n">
         <v>1004</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="C5" s="0" t="s">
-        <v>8</v>
+        <v>22</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="0" t="n">
+        <v>6543210987</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="n">
+      <c r="A6" s="1" t="n">
         <v>1005</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>27</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>5432109876</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" display="johndoe@gmail.com"/>
+    <hyperlink ref="E3" r:id="rId2" display="taochain@gmail.com"/>
+    <hyperlink ref="E4" r:id="rId3" display="husain@outlook.com"/>
+    <hyperlink ref="E5" r:id="rId4" display="vankat@yahoo.com"/>
+    <hyperlink ref="E6" r:id="rId5" display="helen@ukmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
"Added poiji dependency and using it to get data from excel sheet and passing it as a payload to create user and create extent report."
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/CreateUserData.xlsx
+++ b/src/test/resources/testdata/CreateUserData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t xml:space="preserve">Id</t>
   </si>
@@ -43,6 +43,9 @@
     <t xml:space="preserve">Phone</t>
   </si>
   <si>
+    <t xml:space="preserve">RandomId_6</t>
+  </si>
+  <si>
     <t xml:space="preserve">john.doe</t>
   </si>
   <si>
@@ -73,6 +76,9 @@
     <t xml:space="preserve">T12345678</t>
   </si>
   <si>
+    <t xml:space="preserve">RandomId_5</t>
+  </si>
+  <si>
     <t xml:space="preserve">husain.k</t>
   </si>
   <si>
@@ -88,6 +94,9 @@
     <t xml:space="preserve">M12345678</t>
   </si>
   <si>
+    <t xml:space="preserve">RandomId_7</t>
+  </si>
+  <si>
     <t xml:space="preserve">vankat.iyar</t>
   </si>
   <si>
@@ -101,6 +110,9 @@
   </si>
   <si>
     <t xml:space="preserve">V12345678</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RandomId</t>
   </si>
   <si>
     <t xml:space="preserve">helen.kip</t>
@@ -233,9 +245,9 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="18.93"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -262,23 +274,23 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
-        <v>1001</v>
+      <c r="A2" s="1" t="s">
+        <v>7</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>9876543210</v>
@@ -286,91 +298,91 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="n">
-        <v>1002</v>
+        <v>32453</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="G3" s="0" t="n">
         <v>8765432109</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
-        <v>1003</v>
+      <c r="A4" s="1" t="s">
+        <v>18</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G4" s="0" t="n">
         <v>7654321098</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
-        <v>1004</v>
+      <c r="A5" s="1" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G5" s="0" t="n">
         <v>6543210987</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
-        <v>1005</v>
+      <c r="A6" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="G6" s="0" t="n">
         <v>5432109876</v>

</xml_diff>